<commit_message>
- updated LTC4425 breakout with 0402 SMD passives, updated BOM and gerbers
</commit_message>
<xml_diff>
--- a/LTC4425 breakout - BOM.xlsx
+++ b/LTC4425 breakout - BOM.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="LTC4425 breakout - BOM" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LTC4425 breakout - BOM'!$A$1:$G$11</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -139,28 +142,28 @@
     <t>https://hr.mouser.com/ProductDetail/810-CGA2B1X7R1C104K</t>
   </si>
   <si>
-    <t xml:space="preserve">71-RCS040210K0JNED </t>
-  </si>
-  <si>
-    <t>https://hr.mouser.com/ProductDetail/71-RCS040210K0JNED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">71-RCS0402470KJNED </t>
-  </si>
-  <si>
-    <t>https://hr.mouser.com/ProductDetail/Vishay/RCS0402470KJNED?qs=NKmfXavxMazaRTzx%252bYUezA%3d%3d</t>
-  </si>
-  <si>
     <t xml:space="preserve">71-PAT1206E1002BST1 </t>
   </si>
   <si>
     <t>https://hr.mouser.com/ProductDetail/Vishay-Thin-Film/PAT1206E1002BST1?qs=sGAEpiMZZMu61qfTUdNhG0AxE%252b92hZooLdX7Jm3iz7w%3d</t>
   </si>
   <si>
-    <t xml:space="preserve">594-MCS04020C1503FE0 </t>
-  </si>
-  <si>
-    <t>https://hr.mouser.com/ProductDetail/Vishay-Beyschlag/MCS04020C1503FE000?qs=sGAEpiMZZMtlubZbdhIBIMAhWB6%252bRofmgrLcZSglu%252bU%3d</t>
+    <t>667-ERJ-PA2J103X</t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/Panasonic/ERJ-PA2J103X/?qs=sGAEpiMZZMvdGkrng054twEmCE4Hl1aVwYY3whshWPdEaZIYFtkXIA%3d%3d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667-ERJ-PA2D4703X </t>
+  </si>
+  <si>
+    <t xml:space="preserve">667-ERJ-PA2D1503X </t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/Panasonic/ERJ-PA2D1503X?qs=sGAEpiMZZMvdGkrng054t39FRO7iDkA6eGGuNuEw%2fLNtcQIIMUugpA%3d%3d</t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/Panasonic/ERJ-PA2D4703X?qs=sGAEpiMZZMvdGkrng054t39FRO7iDkA6m4gJshzSy97Iz9QkARiOSA%3d%3d</t>
   </si>
 </sst>
 </file>
@@ -1022,14 +1025,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="6.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.88671875" customWidth="1"/>
+    <col min="6" max="6" width="23.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1139,10 +1146,10 @@
         <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1162,10 +1169,10 @@
         <v>21</v>
       </c>
       <c r="F6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1185,10 +1192,10 @@
         <v>21</v>
       </c>
       <c r="F7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1208,10 +1215,10 @@
         <v>21</v>
       </c>
       <c r="F8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1231,10 +1238,10 @@
         <v>21</v>
       </c>
       <c r="F9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1254,10 +1261,10 @@
         <v>21</v>
       </c>
       <c r="F10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1277,24 +1284,23 @@
         <v>21</v>
       </c>
       <c r="F11" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:G11">
+    <sortCondition ref="A2:A11"/>
+  </sortState>
   <hyperlinks>
     <hyperlink ref="G4" r:id="rId1"/>
     <hyperlink ref="G3" r:id="rId2"/>
     <hyperlink ref="G2" r:id="rId3"/>
-    <hyperlink ref="G10" r:id="rId4"/>
-    <hyperlink ref="G11" r:id="rId5"/>
-    <hyperlink ref="G8" r:id="rId6"/>
-    <hyperlink ref="G9" r:id="rId7"/>
-    <hyperlink ref="G5" r:id="rId8"/>
-    <hyperlink ref="G6" r:id="rId9"/>
-    <hyperlink ref="G7" r:id="rId10"/>
+    <hyperlink ref="G5" r:id="rId4"/>
+    <hyperlink ref="G10" r:id="rId5"/>
+    <hyperlink ref="G11" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- corrected passives form factor in BOM
</commit_message>
<xml_diff>
--- a/LTC4425 breakout - BOM.xlsx
+++ b/LTC4425 breakout - BOM.xlsx
@@ -37,12 +37,6 @@
     <t>C2</t>
   </si>
   <si>
-    <t>C-EUC0805</t>
-  </si>
-  <si>
-    <t>C0805</t>
-  </si>
-  <si>
     <t>CAPACITOR, European symbol</t>
   </si>
   <si>
@@ -91,12 +85,6 @@
     <t>150k</t>
   </si>
   <si>
-    <t>R-EU_R0805</t>
-  </si>
-  <si>
-    <t>R0805</t>
-  </si>
-  <si>
     <t>R3</t>
   </si>
   <si>
@@ -164,6 +152,18 @@
   </si>
   <si>
     <t>https://hr.mouser.com/ProductDetail/Panasonic/ERJ-PA2D4703X?qs=sGAEpiMZZMvdGkrng054t39FRO7iDkA6m4gJshzSy97Iz9QkARiOSA%3d%3d</t>
+  </si>
+  <si>
+    <t>R-EU_R0402</t>
+  </si>
+  <si>
+    <t>R0402</t>
+  </si>
+  <si>
+    <t>C-EUC0402</t>
+  </si>
+  <si>
+    <t>C0402</t>
   </si>
 </sst>
 </file>
@@ -676,10 +676,13 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1026,7 +1029,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1057,10 +1060,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1068,226 +1071,226 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>25</v>
+        <v>21</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" t="s">
-        <v>25</v>
+        <v>21</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" t="s">
         <v>24</v>
       </c>
-      <c r="D8" t="s">
-        <v>25</v>
+      <c r="C8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" t="s">
         <v>24</v>
       </c>
-      <c r="D9" t="s">
-        <v>25</v>
+      <c r="C9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" t="s">
-        <v>25</v>
+        <v>16</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" t="s">
-        <v>25</v>
+        <v>16</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="E11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F11" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>